<commit_message>
Added text_editor.py , improved wording in interface and added the project file for the class diagram
</commit_message>
<xml_diff>
--- a/documentation/interface_prototype.xlsx
+++ b/documentation/interface_prototype.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gudmundur\Dropbox\Tölvunarfræði\Verk1\hópverk\verklegtnamskeid1\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\runar\Desktop\verklegtnamskeid1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3D23C7-8B36-40C5-8CC4-47A9B4CA418C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582F3726-1CB6-4442-A157-845C2C2015A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" firstSheet="4" activeTab="10" xr2:uid="{58F8AC2C-8322-4C75-B6AC-E1E52170CA44}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" firstSheet="4" activeTab="5" xr2:uid="{58F8AC2C-8322-4C75-B6AC-E1E52170CA44}"/>
   </bookViews>
   <sheets>
     <sheet name="Grunnur" sheetId="3" r:id="rId1"/>
@@ -33,9 +33,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="58">
   <si>
     <t>NaN air</t>
   </si>
@@ -141,9 +139,6 @@
     <t>(5) Find employee by name</t>
   </si>
   <si>
-    <t>(6) Find pilots by licences</t>
-  </si>
-  <si>
     <t>(7) Show employees on duty</t>
   </si>
   <si>
@@ -201,22 +196,25 @@
     <t xml:space="preserve">(3) Seating capacity:  </t>
   </si>
   <si>
-    <t xml:space="preserve">(2) Kt:  </t>
-  </si>
-  <si>
     <t>(5) Phone:</t>
   </si>
   <si>
-    <t xml:space="preserve">(4) Adress:  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(3) Possition:  </t>
-  </si>
-  <si>
     <t>(6) Mobile:</t>
   </si>
   <si>
     <t>(7) Aiplane licence (pilot only):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3) Position:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2) Social Security Number:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4) Address:  </t>
+  </si>
+  <si>
+    <t>(6) Find pilots by licence</t>
   </si>
 </sst>
 </file>
@@ -326,12 +324,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -339,6 +331,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -660,40 +658,40 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="11" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>16</v>
       </c>
@@ -710,98 +708,98 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
         <v>12</v>
       </c>
@@ -810,7 +808,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
         <v>13</v>
       </c>
@@ -819,7 +817,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -839,17 +837,17 @@
   <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
@@ -858,16 +856,16 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -876,7 +874,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
@@ -893,50 +891,50 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="14" t="s">
-        <v>48</v>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -945,7 +943,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -955,30 +953,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
@@ -987,7 +985,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
@@ -996,7 +994,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1016,18 +1014,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9861426-BE99-41C7-A84D-06F1C964CB91}">
   <dimension ref="B2:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1036,16 +1034,16 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1054,7 +1052,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1071,8 +1069,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="14" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="4"/>
@@ -1080,45 +1078,45 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1127,9 +1125,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1139,32 +1137,32 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="15" t="s">
-        <v>57</v>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
@@ -1173,7 +1171,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
@@ -1182,7 +1180,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1206,40 +1204,40 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="11" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1256,35 +1254,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
         <v>1</v>
@@ -1293,42 +1291,42 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
@@ -1337,7 +1335,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
@@ -1346,7 +1344,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1369,14 +1367,14 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1385,16 +1383,16 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1403,7 +1401,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>16</v>
       </c>
@@ -1420,7 +1418,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
@@ -1429,7 +1427,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1438,7 +1436,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
@@ -1447,7 +1445,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
@@ -1456,7 +1454,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
@@ -1465,7 +1463,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
@@ -1474,7 +1472,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1484,28 +1482,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
@@ -1514,7 +1512,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
@@ -1523,7 +1521,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1544,17 +1542,17 @@
   <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B5:F6"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1563,16 +1561,16 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1581,7 +1579,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1598,7 +1596,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1607,7 +1605,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
@@ -1616,7 +1614,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>29</v>
       </c>
@@ -1625,7 +1623,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>30</v>
       </c>
@@ -1634,7 +1632,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
@@ -1643,18 +1641,18 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1664,30 +1662,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
@@ -1696,7 +1694,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
@@ -1705,7 +1703,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1728,14 +1726,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1744,16 +1742,16 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1762,7 +1760,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1779,55 +1777,55 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1837,28 +1835,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
@@ -1867,7 +1865,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
@@ -1876,7 +1874,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1895,18 +1893,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BDC1B48-829D-4E8B-80EA-B5ED7D32EC90}">
   <dimension ref="B2:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1915,16 +1913,16 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1933,7 +1931,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1950,46 +1948,46 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1998,7 +1996,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -2008,28 +2006,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
@@ -2038,7 +2036,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
@@ -2047,7 +2045,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2070,14 +2068,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
@@ -2086,16 +2084,16 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -2104,7 +2102,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
@@ -2121,21 +2119,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
         <v>10</v>
@@ -2144,32 +2142,32 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -2179,28 +2177,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
@@ -2209,7 +2207,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
@@ -2218,7 +2216,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2240,7 +2238,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2254,14 +2252,14 @@
       <selection activeCell="B15" sqref="B7:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
@@ -2270,16 +2268,16 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -2288,7 +2286,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
@@ -2305,8 +2303,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="14" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="4"/>
@@ -2314,43 +2312,43 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -2359,7 +2357,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -2369,30 +2367,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
@@ -2401,7 +2399,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
@@ -2410,7 +2408,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>

</xml_diff>

<commit_message>
happy path and exel interfacedesign
</commit_message>
<xml_diff>
--- a/documentation/interface_prototype.xlsx
+++ b/documentation/interface_prototype.xlsx
@@ -5,25 +5,31 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\runar\Desktop\verklegtnamskeid1\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gudmundur\Dropbox\Tölvunarfræði\Verk1\hópverk\verklegtnamskeid1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582F3726-1CB6-4442-A157-845C2C2015A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9E5752-998D-4ABE-B23A-34A05DCD89AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" firstSheet="4" activeTab="5" xr2:uid="{58F8AC2C-8322-4C75-B6AC-E1E52170CA44}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" firstSheet="7" activeTab="10" xr2:uid="{58F8AC2C-8322-4C75-B6AC-E1E52170CA44}"/>
   </bookViews>
   <sheets>
     <sheet name="Grunnur" sheetId="3" r:id="rId1"/>
-    <sheet name="Welcome" sheetId="2" r:id="rId2"/>
+    <sheet name="Welcome" sheetId="16" r:id="rId2"/>
     <sheet name="Voyages" sheetId="11" r:id="rId3"/>
     <sheet name="Employees" sheetId="6" r:id="rId4"/>
     <sheet name="Airplanes" sheetId="7" r:id="rId5"/>
     <sheet name="Flight routes" sheetId="9" r:id="rId6"/>
     <sheet name="Quit" sheetId="10" r:id="rId7"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
-    <sheet name="New Flight routes" sheetId="12" r:id="rId9"/>
-    <sheet name="New Airplane" sheetId="13" r:id="rId10"/>
-    <sheet name="New Employee" sheetId="14" r:id="rId11"/>
+    <sheet name="New Flight route" sheetId="12" r:id="rId8"/>
+    <sheet name="New Airplane" sheetId="13" r:id="rId9"/>
+    <sheet name="New Employee" sheetId="14" r:id="rId10"/>
+    <sheet name="New Voyage" sheetId="15" r:id="rId11"/>
+    <sheet name="New Voyage fill" sheetId="30" r:id="rId12"/>
+    <sheet name="New Voy-flight route" sheetId="19" r:id="rId13"/>
+    <sheet name="New Voyage schedule" sheetId="20" r:id="rId14"/>
+    <sheet name="New Voy-airplanes" sheetId="29" r:id="rId15"/>
+    <sheet name="New Voy-pilots" sheetId="21" r:id="rId16"/>
+    <sheet name="New Voy-Flight attendants" sheetId="28" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,37 +39,43 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="120">
   <si>
     <t>NaN air</t>
   </si>
   <si>
-    <t>Welcome screen</t>
-  </si>
-  <si>
-    <t>Employees</t>
-  </si>
-  <si>
-    <t>Voyages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Airplaines   </t>
-  </si>
-  <si>
-    <t>Quit</t>
-  </si>
-  <si>
-    <t>Flight routes</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -145,9 +157,6 @@
     <t>(8) Show employees off duty</t>
   </si>
   <si>
-    <t>(1)New flight route</t>
-  </si>
-  <si>
     <t>(2) Show all flight routes</t>
   </si>
   <si>
@@ -157,18 +166,6 @@
     <t>(N)o</t>
   </si>
   <si>
-    <t xml:space="preserve">(1) Destination:  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2) Id number:  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(3) Contact name:  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4) Emergency phonenumber:  </t>
-  </si>
-  <si>
     <t>(S)ave</t>
   </si>
   <si>
@@ -184,9 +181,6 @@
     <t>(3) Show airplanes in use</t>
   </si>
   <si>
-    <t>New Airplane</t>
-  </si>
-  <si>
     <t xml:space="preserve">(1) Name:  </t>
   </si>
   <si>
@@ -215,13 +209,339 @@
   </si>
   <si>
     <t>(6) Find pilots by licence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1) Country:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2) Destination:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3) Airport id:  </t>
+  </si>
+  <si>
+    <t>New airplane</t>
+  </si>
+  <si>
+    <t>New voyage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(6) Contact name:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(7) Emergency phonenumber:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4) Flight time:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5) Distance from Iceland:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1) Flight route:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    Welcome screen</t>
+  </si>
+  <si>
+    <t>****************************************************************</t>
+  </si>
+  <si>
+    <t>Your Action: v</t>
+  </si>
+  <si>
+    <t>Your Action: 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  20/02/20 12:30  RETURN  20/02/20 18:15</t>
+  </si>
+  <si>
+    <r>
+      <t>New voyage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Flight routes</t>
+    </r>
+  </si>
+  <si>
+    <t>(1) Nuuk</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>1428 km</t>
+  </si>
+  <si>
+    <t>Greenland</t>
+  </si>
+  <si>
+    <t>(2) Kulusuk</t>
+  </si>
+  <si>
+    <t>735 km</t>
+  </si>
+  <si>
+    <t>Faroe islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4) Tingwall </t>
+  </si>
+  <si>
+    <t>Shetland</t>
+  </si>
+  <si>
+    <t>1181 km</t>
+  </si>
+  <si>
+    <t>795 km</t>
+  </si>
+  <si>
+    <t>(5) Longyearbyen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Svalbard </t>
+  </si>
+  <si>
+    <t>1991 km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3) Tórshavn  </t>
+  </si>
+  <si>
+    <t>Choose flight route: 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Destination</t>
+  </si>
+  <si>
+    <t>Longyearbyen</t>
+  </si>
+  <si>
+    <r>
+      <t>New voyage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Voyage schedule</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Return flight date:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Flight departure time:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Return flight departure time:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Flight date:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Flight date (dd/mm/yyyy): 20/12/2019_</t>
+  </si>
+  <si>
+    <t>(2) Voyage schedule:  20/12/2019 12:32  RETURN  20/12/2019 21:18</t>
+  </si>
+  <si>
+    <t>(1) Enola gay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Seat count</t>
+  </si>
+  <si>
+    <t>(2) Bockscar</t>
+  </si>
+  <si>
+    <t>Silverplate B-29</t>
+  </si>
+  <si>
+    <t>Boeing B-29</t>
+  </si>
+  <si>
+    <t>(3) Airplane:   Enola gay</t>
+  </si>
+  <si>
+    <t>(2) Robert A. Lewis</t>
+  </si>
+  <si>
+    <t>(1) Paul Tibbits - captain</t>
+  </si>
+  <si>
+    <t>(3) Charles W. Sweeney - pilot</t>
+  </si>
+  <si>
+    <t>Do you want to add another pilot (y/n): n_</t>
+  </si>
+  <si>
+    <t>(4) Pilots: Paul Tibbits, Charles W. Sweeney</t>
+  </si>
+  <si>
+    <r>
+      <t>New voyage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/Available flight attendants</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">(4) Jassica Whitney Dubroff </t>
+  </si>
+  <si>
+    <t>(1) Billy Baskerville</t>
+  </si>
+  <si>
+    <t>(3) Gianna Bustle</t>
+  </si>
+  <si>
+    <t>(2) Craig Frasure</t>
+  </si>
+  <si>
+    <t>(4) Graham Delucia</t>
+  </si>
+  <si>
+    <t>(5) Jacque Rueter</t>
+  </si>
+  <si>
+    <t>Do you want to add another flight attendants (y/n): n_</t>
+  </si>
+  <si>
+    <t>(6) Juliann March - The cabin manager</t>
+  </si>
+  <si>
+    <t>(5) Flight attendants: Juliann March, Craig Frasure</t>
+  </si>
+  <si>
+    <t>Your Action: s</t>
+  </si>
+  <si>
+    <t>(1) New flight route</t>
+  </si>
+  <si>
+    <t>Choose airplane: 1</t>
+  </si>
+  <si>
+    <r>
+      <t>New voyage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Available airplanes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>New voyage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/L</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>icenced pilots available for Boeing B-29</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">(5) Flight attendants: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4) Pilots: </t>
+  </si>
+  <si>
+    <t>(3) Airplane:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2) Voyage schedule: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +573,13 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -293,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -310,9 +637,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -337,6 +661,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -655,169 +985,169 @@
   <dimension ref="B2:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I13" sqref="I13:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
-        <v>16</v>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="8" t="s">
-        <v>12</v>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -833,168 +1163,176 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4296326D-F91E-49B2-B694-1F6441378A5B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9861426-BE99-41C7-A84D-06F1C964CB91}">
   <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>25</v>
+        <v>10</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
-        <v>47</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="11" t="s">
+        <v>2</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="4"/>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="J12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>12</v>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1011,176 +1349,1533 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9861426-BE99-41C7-A84D-06F1C964CB91}">
-  <dimension ref="B2:J18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE6D392-4818-4313-B4A9-8B9A827901D3}">
+  <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>26</v>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+        <v>119</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
-        <v>56</v>
+        <v>117</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C22" cm="1">
+        <f t="array" aca="1" ref="C22" ca="1">+B22:C29</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81890274-58F6-4C8E-BE76-5A1856502A26}">
+  <dimension ref="B2:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="K21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C22" cm="1">
+        <f t="array" aca="1" ref="C22" ca="1">+B22:C29</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAA3177-9EBF-4555-9CB2-FBAC80F943B3}">
+  <dimension ref="B2:J22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
-        <v>52</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="J12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="4"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C22" cm="1">
+        <f t="array" aca="1" ref="C22" ca="1">+B22:C29</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED89526-53A9-40CA-A7FD-C33A4CB15F1F}">
+  <dimension ref="B2:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="J12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="13" t="s">
-        <v>53</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="4"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="K21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C22" cm="1">
+        <f t="array" aca="1" ref="C22" ca="1">+B22:C29</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79EB7330-DA3F-440B-AE83-BBC2DD990CC8}">
+  <dimension ref="B2:J22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="4">
+        <v>146</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="4">
+        <v>80</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="16"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="J12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="4"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C22" cm="1">
+        <f t="array" aca="1" ref="C22" ca="1">+B22:C29</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EEF1AB-A6A0-4B2D-B42D-FE3444AD8CE2}">
+  <dimension ref="B2:J22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="J12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="4"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C22" cm="1">
+        <f t="array" aca="1" ref="C22" ca="1">+B22:C29</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C39595B-449E-41F1-A315-53AB54A66683}">
+  <dimension ref="B2:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B12" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="4"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C22" cm="1">
+        <f t="array" aca="1" ref="C22" ca="1">+B22:C29</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J9:J13">
+    <sortCondition ref="J13"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA1681F-2B1A-43EA-B499-280E5CE62760}">
+  <dimension ref="B2:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="J12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
-        <v>42</v>
-      </c>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>12</v>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1192,170 +2887,7 @@
     <mergeCell ref="B3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88E0630-9D49-4B95-BADC-F26A9BBAD2D6}">
-  <dimension ref="B2:F18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:D3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1364,164 +2896,164 @@
   <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
-        <v>16</v>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="J12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>12</v>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1542,168 +3074,168 @@
   <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>26</v>
+        <v>10</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="J12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>12</v>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1726,155 +3258,155 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="J12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>12</v>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1893,159 +3425,159 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BDC1B48-829D-4E8B-80EA-B5ED7D32EC90}">
   <dimension ref="B2:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="J12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>12</v>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2068,155 +3600,155 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4"/>
-      <c r="C10" s="11" t="s">
-        <v>36</v>
+      <c r="C10" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="J12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>12</v>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2233,182 +3765,176 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58894651-A245-4CC4-BF2B-18BDA26737AC}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F50BAE-02E0-4D0E-B7FF-7309E243D1EE}">
   <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B7:B15"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="11" t="s">
+        <v>3</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="J12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>12</v>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2423,4 +3949,182 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4296326D-F91E-49B2-B694-1F6441378A5B}">
+  <dimension ref="B2:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="J12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed the use cases and added one option in the airplane menu
</commit_message>
<xml_diff>
--- a/documentation/interface_prototype.xlsx
+++ b/documentation/interface_prototype.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gudmundur\Dropbox\Tölvunarfræði\Verk1\hópverk\verklegtnamskeid1\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\runar\Desktop\verklegtnamskeid1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45B5FCA-B2D3-48D0-BA25-8E197DB67DF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333ED6F4-EB46-40E1-86CE-929518E34E65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" firstSheet="5" activeTab="10" xr2:uid="{58F8AC2C-8322-4C75-B6AC-E1E52170CA44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{58F8AC2C-8322-4C75-B6AC-E1E52170CA44}"/>
   </bookViews>
   <sheets>
     <sheet name="Grunnur" sheetId="3" r:id="rId1"/>
@@ -39,9 +39,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -49,14 +47,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -71,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="119">
   <si>
     <t>NaN air</t>
   </si>
@@ -529,6 +527,9 @@
   </si>
   <si>
     <t xml:space="preserve">(4) Jessica Whitney Dubroff </t>
+  </si>
+  <si>
+    <t>(4) Show all airplane types</t>
   </si>
 </sst>
 </file>
@@ -982,13 +983,13 @@
       <selection activeCell="I13" sqref="I13:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>32</v>
       </c>
@@ -997,7 +998,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
@@ -1006,7 +1007,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>32</v>
       </c>
@@ -1015,7 +1016,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -1032,98 +1033,98 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>6</v>
       </c>
@@ -1132,7 +1133,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
         <v>7</v>
       </c>
@@ -1141,7 +1142,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1164,14 +1165,14 @@
       <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1180,7 +1181,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1189,7 +1190,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1198,7 +1199,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1215,7 +1216,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>2</v>
       </c>
@@ -1224,7 +1225,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>36</v>
       </c>
@@ -1233,7 +1234,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>43</v>
       </c>
@@ -1242,7 +1243,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>42</v>
       </c>
@@ -1251,7 +1252,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>44</v>
       </c>
@@ -1260,7 +1261,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>39</v>
       </c>
@@ -1271,7 +1272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
@@ -1283,7 +1284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
         <v>41</v>
       </c>
@@ -1292,14 +1293,14 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
@@ -1308,7 +1309,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -1317,7 +1318,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -1326,7 +1327,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1346,18 +1347,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE6D392-4818-4313-B4A9-8B9A827901D3}">
   <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -1366,7 +1367,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1375,7 +1376,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -1384,7 +1385,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -1401,7 +1402,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>50</v>
       </c>
@@ -1410,7 +1411,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>55</v>
       </c>
@@ -1419,7 +1420,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>115</v>
       </c>
@@ -1428,7 +1429,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>114</v>
       </c>
@@ -1437,7 +1438,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>113</v>
       </c>
@@ -1446,7 +1447,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>112</v>
       </c>
@@ -1457,28 +1458,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
@@ -1487,7 +1488,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -1496,7 +1497,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -1505,21 +1506,21 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C22" cm="1">
-        <f t="array" aca="1" ref="C22" ca="1">+B22:C29</f>
+        <f t="array" ref="C22">+B22:C29</f>
         <v>0</v>
       </c>
     </row>
@@ -1540,14 +1541,14 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -1556,7 +1557,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1565,7 +1566,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -1574,7 +1575,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -1591,7 +1592,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>50</v>
       </c>
@@ -1600,7 +1601,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>55</v>
       </c>
@@ -1611,7 +1612,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>85</v>
       </c>
@@ -1620,7 +1621,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>93</v>
       </c>
@@ -1629,7 +1630,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>98</v>
       </c>
@@ -1638,7 +1639,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>106</v>
       </c>
@@ -1649,28 +1650,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
@@ -1679,7 +1680,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -1688,7 +1689,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>107</v>
       </c>
@@ -1697,26 +1698,26 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="K21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C22" cm="1">
-        <f t="array" aca="1" ref="C22" ca="1">+B22:C29</f>
+        <f t="array" ref="C22">+B22:C29</f>
         <v>0</v>
       </c>
     </row>
@@ -1737,16 +1738,16 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -1755,7 +1756,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1764,7 +1765,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -1773,7 +1774,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -1790,7 +1791,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>59</v>
       </c>
@@ -1799,7 +1800,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>77</v>
       </c>
@@ -1812,7 +1813,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>60</v>
       </c>
@@ -1825,7 +1826,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>65</v>
       </c>
@@ -1838,7 +1839,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>75</v>
       </c>
@@ -1851,7 +1852,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>68</v>
       </c>
@@ -1866,7 +1867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>72</v>
       </c>
@@ -1882,14 +1883,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1898,14 +1899,14 @@
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -1914,7 +1915,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>76</v>
       </c>
@@ -1923,16 +1924,16 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C22" cm="1">
-        <f t="array" aca="1" ref="C22" ca="1">+B22:C29</f>
+        <f t="array" ref="C22">+B22:C29</f>
         <v>0</v>
       </c>
     </row>
@@ -1954,14 +1955,14 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -1970,7 +1971,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1979,7 +1980,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -1988,7 +1989,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -2005,7 +2006,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>79</v>
       </c>
@@ -2014,7 +2015,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>83</v>
       </c>
@@ -2023,7 +2024,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>81</v>
       </c>
@@ -2032,7 +2033,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>80</v>
       </c>
@@ -2041,7 +2042,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>82</v>
       </c>
@@ -2050,7 +2051,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -2059,7 +2060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -2069,28 +2070,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -2099,7 +2100,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>84</v>
       </c>
@@ -2108,21 +2109,21 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="K21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C22" cm="1">
-        <f t="array" aca="1" ref="C22" ca="1">+B22:C29</f>
+        <f t="array" ref="C22">+B22:C29</f>
         <v>0</v>
       </c>
     </row>
@@ -2143,16 +2144,16 @@
       <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -2161,7 +2162,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -2170,7 +2171,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -2179,7 +2180,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -2196,7 +2197,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>110</v>
       </c>
@@ -2205,7 +2206,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>87</v>
       </c>
@@ -2218,7 +2219,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>86</v>
       </c>
@@ -2231,7 +2232,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>90</v>
       </c>
@@ -2244,14 +2245,14 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="14"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -2260,7 +2261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -2270,14 +2271,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2286,14 +2287,14 @@
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -2302,7 +2303,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>109</v>
       </c>
@@ -2311,16 +2312,16 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C22" cm="1">
-        <f t="array" aca="1" ref="C22" ca="1">+B22:C29</f>
+        <f t="array" ref="C22">+B22:C29</f>
         <v>0</v>
       </c>
     </row>
@@ -2341,16 +2342,16 @@
       <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -2359,7 +2360,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -2368,7 +2369,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -2377,7 +2378,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -2394,7 +2395,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>111</v>
       </c>
@@ -2403,7 +2404,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>87</v>
       </c>
@@ -2412,7 +2413,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
         <v>95</v>
       </c>
@@ -2421,7 +2422,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>94</v>
       </c>
@@ -2430,7 +2431,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
         <v>96</v>
       </c>
@@ -2439,7 +2440,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>117</v>
       </c>
@@ -2450,7 +2451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -2460,14 +2461,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2476,14 +2477,14 @@
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -2492,7 +2493,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>97</v>
       </c>
@@ -2501,16 +2502,16 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C22" cm="1">
-        <f t="array" aca="1" ref="C22" ca="1">+B22:C29</f>
+        <f t="array" ref="C22">+B22:C29</f>
         <v>0</v>
       </c>
     </row>
@@ -2531,16 +2532,16 @@
       <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -2549,7 +2550,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -2558,7 +2559,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -2567,7 +2568,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -2584,7 +2585,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>99</v>
       </c>
@@ -2593,7 +2594,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>87</v>
       </c>
@@ -2602,7 +2603,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>100</v>
       </c>
@@ -2611,7 +2612,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>102</v>
       </c>
@@ -2620,7 +2621,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>101</v>
       </c>
@@ -2629,7 +2630,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>103</v>
       </c>
@@ -2640,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>104</v>
       </c>
@@ -2649,7 +2650,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="14" t="s">
         <v>105</v>
       </c>
@@ -2658,7 +2659,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2667,14 +2668,14 @@
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -2683,7 +2684,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>116</v>
       </c>
@@ -2692,16 +2693,16 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C22" cm="1">
-        <f t="array" aca="1" ref="C22" ca="1">+B22:C29</f>
+        <f t="array" ref="C22">+B22:C29</f>
         <v>0</v>
       </c>
     </row>
@@ -2725,14 +2726,14 @@
       <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -2741,7 +2742,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -2750,7 +2751,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -2759,7 +2760,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -2776,35 +2777,35 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
         <v>56</v>
@@ -2813,14 +2814,14 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -2830,28 +2831,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -2860,7 +2861,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -2869,7 +2870,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2893,14 +2894,14 @@
       <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -2909,7 +2910,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -2918,7 +2919,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -2927,7 +2928,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -2944,7 +2945,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
@@ -2953,7 +2954,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
@@ -2962,7 +2963,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
@@ -2971,7 +2972,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
@@ -2980,7 +2981,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
@@ -2989,7 +2990,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
@@ -2998,7 +2999,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -3008,28 +3009,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -3038,7 +3039,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -3047,7 +3048,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3071,14 +3072,14 @@
       <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -3087,7 +3088,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -3096,7 +3097,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -3105,7 +3106,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -3122,7 +3123,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
@@ -3131,7 +3132,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
@@ -3140,7 +3141,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>23</v>
       </c>
@@ -3149,7 +3150,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
@@ -3158,7 +3159,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>25</v>
       </c>
@@ -3167,7 +3168,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>45</v>
       </c>
@@ -3176,7 +3177,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>26</v>
       </c>
@@ -3188,7 +3189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
@@ -3197,21 +3198,21 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -3220,7 +3221,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -3229,7 +3230,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3248,18 +3249,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A78556-8469-4E53-8340-EC30A018C2D7}">
   <dimension ref="B2:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -3268,7 +3269,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -3277,7 +3278,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -3286,7 +3287,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -3303,7 +3304,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>33</v>
       </c>
@@ -3312,7 +3313,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
@@ -3321,7 +3322,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>35</v>
       </c>
@@ -3330,28 +3331,30 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="4"/>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -3361,28 +3364,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -3391,7 +3394,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -3400,7 +3403,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3423,14 +3426,14 @@
       <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -3439,7 +3442,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -3448,7 +3451,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -3457,7 +3460,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -3474,7 +3477,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>108</v>
       </c>
@@ -3483,7 +3486,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
@@ -3492,28 +3495,28 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -3522,7 +3525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -3532,28 +3535,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -3562,7 +3565,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -3571,7 +3574,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3594,14 +3597,14 @@
       <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -3610,7 +3613,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -3619,7 +3622,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -3628,7 +3631,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -3645,21 +3648,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
         <v>4</v>
@@ -3668,14 +3671,14 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="10" t="s">
         <v>29</v>
@@ -3686,14 +3689,14 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -3703,28 +3706,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -3733,7 +3736,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -3742,7 +3745,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3766,14 +3769,14 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -3782,7 +3785,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -3791,7 +3794,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -3800,7 +3803,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -3817,7 +3820,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>3</v>
       </c>
@@ -3826,7 +3829,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>46</v>
       </c>
@@ -3835,7 +3838,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>47</v>
       </c>
@@ -3844,7 +3847,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>48</v>
       </c>
@@ -3853,7 +3856,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>53</v>
       </c>
@@ -3862,7 +3865,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>54</v>
       </c>
@@ -3873,7 +3876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>51</v>
       </c>
@@ -3885,7 +3888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>52</v>
       </c>
@@ -3894,14 +3897,14 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
@@ -3910,7 +3913,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -3919,7 +3922,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -3928,7 +3931,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3953,14 +3956,14 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="2" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -3969,7 +3972,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -3978,7 +3981,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -3987,7 +3990,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -4004,7 +4007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>49</v>
       </c>
@@ -4013,7 +4016,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>36</v>
       </c>
@@ -4022,7 +4025,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>37</v>
       </c>
@@ -4031,7 +4034,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>38</v>
       </c>
@@ -4040,14 +4043,14 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -4056,7 +4059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -4066,21 +4069,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
@@ -4089,7 +4092,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -4098,7 +4101,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -4107,7 +4110,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>

</xml_diff>

<commit_message>
Interface prototype fixed wording
</commit_message>
<xml_diff>
--- a/documentation/interface_prototype.xlsx
+++ b/documentation/interface_prototype.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\runar\Desktop\verklegtnamskeid1\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patti\Desktop\Verk nám\verklegtnamskeid1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333ED6F4-EB46-40E1-86CE-929518E34E65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCA0B09-C562-46F1-9910-98EE7A302B9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{58F8AC2C-8322-4C75-B6AC-E1E52170CA44}"/>
+    <workbookView xWindow="5340" yWindow="120" windowWidth="13820" windowHeight="6000" firstSheet="13" activeTab="16" xr2:uid="{58F8AC2C-8322-4C75-B6AC-E1E52170CA44}"/>
   </bookViews>
   <sheets>
     <sheet name="Grunnur" sheetId="3" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="120">
   <si>
     <t>NaN air</t>
   </si>
@@ -485,6 +485,30 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">(5) Flight attendants: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4) Pilots: </t>
+  </si>
+  <si>
+    <t>(3) Airplane:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2) Voyage schedule: </t>
+  </si>
+  <si>
+    <t>Do you want to add another flight attendant (y/n): n_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4) Jessica Whitney Dubroff </t>
+  </si>
+  <si>
+    <t>(4) Show all airplane types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(F)light routes </t>
+  </si>
+  <si>
     <r>
       <t>New voyage</t>
     </r>
@@ -507,29 +531,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>icenced pilots available for Boeing B-29</t>
+      <t>icensed pilots available for Boeing B-29</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">(5) Flight attendants: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4) Pilots: </t>
-  </si>
-  <si>
-    <t>(3) Airplane:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2) Voyage schedule: </t>
-  </si>
-  <si>
-    <t>Do you want to add another flight attendant (y/n): n_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4) Jessica Whitney Dubroff </t>
-  </si>
-  <si>
-    <t>(4) Show all airplane types</t>
   </si>
 </sst>
 </file>
@@ -980,16 +983,16 @@
   <dimension ref="B2:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13:I14"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>32</v>
       </c>
@@ -998,7 +1001,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1010,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>32</v>
       </c>
@@ -1016,7 +1019,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -1033,98 +1036,98 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="7" t="s">
         <v>6</v>
       </c>
@@ -1133,7 +1136,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="4" t="s">
         <v>7</v>
       </c>
@@ -1142,7 +1145,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1162,17 +1165,17 @@
   <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F18"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1181,7 +1184,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1190,7 +1193,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1199,7 +1202,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
         <v>2</v>
       </c>
@@ -1225,7 +1228,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>36</v>
       </c>
@@ -1234,7 +1237,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>43</v>
       </c>
@@ -1243,7 +1246,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>42</v>
       </c>
@@ -1252,7 +1255,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>44</v>
       </c>
@@ -1261,7 +1264,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>39</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
@@ -1284,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="12" t="s">
         <v>41</v>
       </c>
@@ -1293,14 +1296,14 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
@@ -1309,7 +1312,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -1318,7 +1321,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -1327,7 +1330,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1351,14 +1354,14 @@
       <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -1367,7 +1370,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1376,7 +1379,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -1385,7 +1388,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -1402,7 +1405,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
         <v>50</v>
       </c>
@@ -1411,7 +1414,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>55</v>
       </c>
@@ -1420,36 +1423,36 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="13"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1458,28 +1461,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
@@ -1488,7 +1491,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -1497,7 +1500,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -1506,19 +1509,19 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C22" cm="1">
         <f t="array" ref="C22">+B22:C29</f>
         <v>0</v>
@@ -1541,14 +1544,14 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -1557,7 +1560,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1566,7 +1569,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -1575,7 +1578,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -1592,7 +1595,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
         <v>50</v>
       </c>
@@ -1601,7 +1604,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>55</v>
       </c>
@@ -1612,7 +1615,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>85</v>
       </c>
@@ -1621,7 +1624,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>93</v>
       </c>
@@ -1630,7 +1633,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>98</v>
       </c>
@@ -1639,7 +1642,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>106</v>
       </c>
@@ -1650,28 +1653,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
@@ -1680,7 +1683,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -1689,7 +1692,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>107</v>
       </c>
@@ -1698,24 +1701,24 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
       <c r="K21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C22" cm="1">
         <f t="array" ref="C22">+B22:C29</f>
         <v>0</v>
@@ -1738,16 +1741,16 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -1756,7 +1759,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1765,7 +1768,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -1774,7 +1777,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -1791,7 +1794,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
         <v>59</v>
       </c>
@@ -1800,7 +1803,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>77</v>
       </c>
@@ -1813,7 +1816,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>60</v>
       </c>
@@ -1826,7 +1829,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>65</v>
       </c>
@@ -1839,7 +1842,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>75</v>
       </c>
@@ -1852,7 +1855,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>68</v>
       </c>
@@ -1867,7 +1870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
         <v>72</v>
       </c>
@@ -1883,14 +1886,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1899,14 +1902,14 @@
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -1915,7 +1918,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>76</v>
       </c>
@@ -1924,14 +1927,14 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C22" cm="1">
         <f t="array" ref="C22">+B22:C29</f>
         <v>0</v>
@@ -1955,14 +1958,14 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -1971,7 +1974,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1980,7 +1983,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -1989,7 +1992,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -2006,7 +2009,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
         <v>79</v>
       </c>
@@ -2015,7 +2018,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>83</v>
       </c>
@@ -2024,7 +2027,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>81</v>
       </c>
@@ -2033,7 +2036,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>80</v>
       </c>
@@ -2042,7 +2045,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>82</v>
       </c>
@@ -2051,7 +2054,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -2060,7 +2063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -2070,28 +2073,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -2100,7 +2103,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>84</v>
       </c>
@@ -2109,19 +2112,19 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
       <c r="K21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C22" cm="1">
         <f t="array" ref="C22">+B22:C29</f>
         <v>0</v>
@@ -2144,16 +2147,16 @@
       <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -2162,7 +2165,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -2171,7 +2174,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -2180,7 +2183,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -2197,7 +2200,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
         <v>110</v>
       </c>
@@ -2206,7 +2209,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>87</v>
       </c>
@@ -2219,7 +2222,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>86</v>
       </c>
@@ -2232,7 +2235,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>90</v>
       </c>
@@ -2245,14 +2248,14 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="14"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -2261,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -2271,14 +2274,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2287,14 +2290,14 @@
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -2303,7 +2306,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>109</v>
       </c>
@@ -2312,14 +2315,14 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C22" cm="1">
         <f t="array" ref="C22">+B22:C29</f>
         <v>0</v>
@@ -2339,19 +2342,19 @@
   <dimension ref="B2:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -2360,7 +2363,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -2369,7 +2372,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -2378,7 +2381,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -2395,16 +2398,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>87</v>
       </c>
@@ -2413,7 +2416,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="14" t="s">
         <v>95</v>
       </c>
@@ -2422,7 +2425,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>94</v>
       </c>
@@ -2431,7 +2434,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="14" t="s">
         <v>96</v>
       </c>
@@ -2440,9 +2443,9 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -2451,7 +2454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -2461,14 +2464,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2477,14 +2480,14 @@
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -2493,7 +2496,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>97</v>
       </c>
@@ -2502,14 +2505,14 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C22" cm="1">
         <f t="array" ref="C22">+B22:C29</f>
         <v>0</v>
@@ -2528,20 +2531,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C39595B-449E-41F1-A315-53AB54A66683}">
   <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -2550,7 +2553,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -2559,7 +2562,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -2568,7 +2571,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -2585,7 +2588,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
         <v>99</v>
       </c>
@@ -2594,7 +2597,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>87</v>
       </c>
@@ -2603,7 +2606,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>100</v>
       </c>
@@ -2612,7 +2615,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>102</v>
       </c>
@@ -2621,7 +2624,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>101</v>
       </c>
@@ -2630,7 +2633,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>103</v>
       </c>
@@ -2641,7 +2644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
         <v>104</v>
       </c>
@@ -2650,7 +2653,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="14" t="s">
         <v>105</v>
       </c>
@@ -2659,7 +2662,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2668,14 +2671,14 @@
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -2684,23 +2687,23 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C22" cm="1">
         <f t="array" ref="C22">+B22:C29</f>
         <v>0</v>
@@ -2726,14 +2729,14 @@
       <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -2742,7 +2745,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -2751,7 +2754,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
@@ -2760,7 +2763,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -2777,35 +2780,35 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
         <v>56</v>
@@ -2814,14 +2817,14 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -2831,28 +2834,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -2861,7 +2864,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -2870,7 +2873,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2894,14 +2897,14 @@
       <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
@@ -2910,7 +2913,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -2919,7 +2922,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -2928,7 +2931,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
@@ -2945,7 +2948,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
@@ -2954,7 +2957,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
@@ -2963,7 +2966,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
@@ -2972,7 +2975,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
@@ -2981,7 +2984,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
@@ -2990,7 +2993,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
@@ -2999,7 +3002,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -3009,28 +3012,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -3039,7 +3042,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -3048,7 +3051,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3069,17 +3072,17 @@
   <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F18"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -3088,7 +3091,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -3097,7 +3100,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -3106,7 +3109,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -3123,7 +3126,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
@@ -3132,7 +3135,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
@@ -3141,7 +3144,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>23</v>
       </c>
@@ -3150,7 +3153,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
@@ -3159,7 +3162,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>25</v>
       </c>
@@ -3168,7 +3171,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>45</v>
       </c>
@@ -3177,7 +3180,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
         <v>26</v>
       </c>
@@ -3189,7 +3192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
@@ -3198,21 +3201,21 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -3221,7 +3224,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -3230,7 +3233,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3249,18 +3252,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A78556-8469-4E53-8340-EC30A018C2D7}">
   <dimension ref="B2:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -3269,7 +3272,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -3278,7 +3281,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -3287,7 +3290,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -3298,13 +3301,13 @@
         <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>11</v>
+        <v>118</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
         <v>33</v>
       </c>
@@ -3313,7 +3316,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
@@ -3322,7 +3325,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>35</v>
       </c>
@@ -3331,30 +3334,30 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -3364,28 +3367,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -3394,7 +3397,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -3403,7 +3406,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3423,17 +3426,17 @@
   <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F18"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -3442,7 +3445,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -3451,7 +3454,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -3460,7 +3463,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -3477,7 +3480,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
         <v>108</v>
       </c>
@@ -3486,7 +3489,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
@@ -3495,28 +3498,28 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -3525,7 +3528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -3535,28 +3538,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -3565,7 +3568,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -3574,7 +3577,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3594,17 +3597,17 @@
   <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F18"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -3613,7 +3616,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -3622,7 +3625,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -3631,7 +3634,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -3648,21 +3651,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
         <v>4</v>
@@ -3671,14 +3674,14 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4"/>
       <c r="C10" s="10" t="s">
         <v>29</v>
@@ -3689,14 +3692,14 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -3706,28 +3709,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -3736,7 +3739,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -3745,7 +3748,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3769,14 +3772,14 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -3785,7 +3788,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -3794,7 +3797,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -3803,7 +3806,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -3820,7 +3823,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
         <v>3</v>
       </c>
@@ -3829,7 +3832,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>46</v>
       </c>
@@ -3838,7 +3841,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>47</v>
       </c>
@@ -3847,7 +3850,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>48</v>
       </c>
@@ -3856,7 +3859,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>53</v>
       </c>
@@ -3865,7 +3868,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>54</v>
       </c>
@@ -3876,7 +3879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
         <v>51</v>
       </c>
@@ -3888,7 +3891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
         <v>52</v>
       </c>
@@ -3897,14 +3900,14 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
@@ -3913,7 +3916,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -3922,7 +3925,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -3931,7 +3934,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3956,14 +3959,14 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -3972,7 +3975,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -3981,7 +3984,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -3990,7 +3993,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -4007,7 +4010,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
         <v>49</v>
       </c>
@@ -4016,7 +4019,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>36</v>
       </c>
@@ -4025,7 +4028,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>37</v>
       </c>
@@ -4034,7 +4037,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>38</v>
       </c>
@@ -4043,14 +4046,14 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -4059,7 +4062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -4069,21 +4072,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
@@ -4092,7 +4095,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
@@ -4101,7 +4104,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -4110,7 +4113,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>

</xml_diff>